<commit_message>
pass param search to controller
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac cu dan toc.xlsx
+++ b/eCert/Uploads/Nhac cu dan toc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -56,9 +56,6 @@
     <t>AvgMark</t>
   </si>
   <si>
-    <t>HE130589</t>
-  </si>
-  <si>
     <t>Hà Phúc Trí</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>Mông</t>
   </si>
   <si>
-    <t>HE130475</t>
-  </si>
-  <si>
     <t>Nguyễn Ngọc Hải</t>
   </si>
   <si>
@@ -116,9 +110,6 @@
     <t>ĐH200303</t>
   </si>
   <si>
-    <t>HE123456</t>
-  </si>
-  <si>
     <t>23/08/1999</t>
   </si>
   <si>
@@ -129,6 +120,9 @@
   </si>
   <si>
     <t>Sáo</t>
+  </si>
+  <si>
+    <t>HE130576</t>
   </si>
 </sst>
 </file>
@@ -449,7 +443,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +492,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -509,37 +503,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
       <c r="J2">
         <v>8.1</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -547,37 +541,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
       </c>
       <c r="J3">
         <v>7.5</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -585,37 +579,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
       <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
       </c>
       <c r="J4">
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>